<commit_message>
Ver. 0.4 *Finished DocsWork class (added layout for second document) *Fixed some bugs (programm no longer tries to read "phone" from excel table as datetime)
</commit_message>
<xml_diff>
--- a/Журнал отлова (full).xlsx
+++ b/Журнал отлова (full).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pshar\source\repos\DogSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26909607-E5BE-4193-82F4-4FE9C8A623D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D75FB0-538D-4A10-BE7A-4D10153FBB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="786">
   <si>
     <t>Куратор</t>
   </si>
@@ -2380,6 +2380,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Мультикан 8</t>
   </si>
 </sst>
 </file>
@@ -11730,7 +11733,9 @@
       <c r="N150" s="12" t="s">
         <v>776</v>
       </c>
-      <c r="O150" s="12"/>
+      <c r="O150" s="12" t="s">
+        <v>785</v>
+      </c>
       <c r="P150" s="15" t="s">
         <v>777</v>
       </c>

</xml_diff>